<commit_message>
MQ source connector with TLS and Authentication
</commit_message>
<xml_diff>
--- a/doc/Functions.xlsx
+++ b/doc/Functions.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CurrentProjects\CP4I\Installation\cp4i-install\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C9A6E1-386F-418D-8842-C8633DCD2184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01902BFC-3B52-4A3F-B60F-FA0CC329DC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57615" yWindow="5175" windowWidth="23505" windowHeight="13935" xr2:uid="{1B9FF1CA-3A2B-40EE-98A9-4DCC44A71825}"/>
+    <workbookView xWindow="51024" yWindow="1704" windowWidth="21828" windowHeight="12948" tabRatio="483" xr2:uid="{1B9FF1CA-3A2B-40EE-98A9-4DCC44A71825}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$130</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$133</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="147">
   <si>
     <t>lib.sh</t>
   </si>
@@ -473,10 +473,16 @@
     <t>Count of Categorie</t>
   </si>
   <si>
-    <t>proovision.sh</t>
-  </si>
-  <si>
     <t>provision_cluster-v2.sh</t>
+  </si>
+  <si>
+    <t>create_generic_secret</t>
+  </si>
+  <si>
+    <t>create_self_signed_issuer</t>
+  </si>
+  <si>
+    <t>helm_install</t>
   </si>
 </sst>
 </file>
@@ -520,14 +526,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,16 +551,17 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Arnauld Desprets" refreshedDate="45918.596812962962" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="130" xr:uid="{763A97D6-A164-4CE7-859E-DD231018B5DF}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Arnauld Desprets" refreshedDate="45925.429378703702" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="133" xr:uid="{763A97D6-A164-4CE7-859E-DD231018B5DF}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:C1048576" sheet="Sheet1"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="File" numFmtId="0">
-      <sharedItems containsBlank="1" count="4">
+      <sharedItems containsBlank="1" count="5">
         <s v="lib.sh"/>
-        <s v="proovision.sh"/>
+        <s v="provision_cluster-v2.sh"/>
         <m/>
+        <s v="proovision.sh" u="1"/>
         <s v="install_sftp" u="1"/>
       </sharedItems>
     </cacheField>
@@ -582,7 +588,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="130">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="133">
   <r>
     <x v="0"/>
     <s v="install_mq_k8s"/>
@@ -912,6 +918,21 @@
     <x v="0"/>
     <s v="adapt_file"/>
     <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="create_self_signed_issuer"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="create_generic_secret"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="helm_install"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="0"/>
@@ -1237,14 +1258,15 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{84E5FE0C-A8DF-4E88-AA47-A1A75C172A4E}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="E3:H10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{84E5FE0C-A8DF-4E88-AA47-A1A75C172A4E}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="F3:I10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item m="1" x="3"/>
+      <items count="6">
+        <item m="1" x="4"/>
         <item x="0"/>
         <item h="1" x="2"/>
+        <item h="1" m="1" x="3"/>
         <item x="1"/>
         <item t="default"/>
       </items>
@@ -1293,7 +1315,7 @@
       <x v="1"/>
     </i>
     <i>
-      <x v="3"/>
+      <x v="4"/>
     </i>
     <i t="grand">
       <x/>
@@ -1631,26 +1653,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C69EDCCF-BBE4-4988-BD44-ED3F6C7FAE7E}">
-  <dimension ref="A1:H130"/>
+  <dimension ref="A1:I133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C68" sqref="C68:C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.7890625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.26171875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5234375" customWidth="1"/>
-    <col min="5" max="5" width="16.89453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.3125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.3125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.26171875" customWidth="1"/>
+    <col min="6" max="6" width="15.68359375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.9453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.41796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.9453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>134</v>
       </c>
@@ -1663,8 +1686,9 @@
       <c r="D1" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1675,7 +1699,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1685,14 +1709,14 @@
       <c r="C3" t="s">
         <v>130</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1702,20 +1726,20 @@
       <c r="C4" t="s">
         <v>130</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="F4" t="s">
-        <v>0</v>
-      </c>
       <c r="G4" t="s">
-        <v>143</v>
+        <v>0</v>
       </c>
       <c r="H4" t="s">
+        <v>143</v>
+      </c>
+      <c r="I4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1725,20 +1749,20 @@
       <c r="C5" t="s">
         <v>130</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
         <v>1</v>
       </c>
-      <c r="G5" s="4">
-        <v>1</v>
-      </c>
-      <c r="H5" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="I5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1748,18 +1772,17 @@
       <c r="C6" t="s">
         <v>130</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4">
+      <c r="H6">
         <v>15</v>
       </c>
-      <c r="H6" s="4">
+      <c r="I6">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1769,20 +1792,20 @@
       <c r="C7" t="s">
         <v>130</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G7">
         <v>20</v>
       </c>
-      <c r="G7" s="4">
+      <c r="H7">
         <v>35</v>
       </c>
-      <c r="H7" s="4">
+      <c r="I7">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1792,20 +1815,20 @@
       <c r="C8" t="s">
         <v>130</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F8" s="4">
-        <v>29</v>
-      </c>
-      <c r="G8" s="4">
+      <c r="F8" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G8">
+        <v>30</v>
+      </c>
+      <c r="H8">
         <v>3</v>
       </c>
-      <c r="H8" s="4">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="I8">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1815,20 +1838,20 @@
       <c r="C9" t="s">
         <v>130</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="F9" s="4">
+      <c r="G9">
         <v>23</v>
       </c>
-      <c r="G9" s="4">
+      <c r="H9">
         <v>2</v>
       </c>
-      <c r="H9" s="4">
+      <c r="I9">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1838,20 +1861,20 @@
       <c r="C10" t="s">
         <v>130</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="F10" s="4">
-        <v>73</v>
-      </c>
-      <c r="G10" s="4">
+      <c r="G10">
+        <v>76</v>
+      </c>
+      <c r="H10">
         <v>56</v>
       </c>
-      <c r="H10" s="4">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="I10">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1862,7 +1885,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1873,7 +1896,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1884,7 +1907,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1895,7 +1918,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1906,7 +1929,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -2483,7 +2506,7 @@
         <v>0</v>
       </c>
       <c r="B68" t="s">
-        <v>67</v>
+        <v>145</v>
       </c>
       <c r="C68" t="s">
         <v>137</v>
@@ -2494,10 +2517,10 @@
         <v>0</v>
       </c>
       <c r="B69" t="s">
-        <v>68</v>
+        <v>144</v>
       </c>
       <c r="C69" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -2505,10 +2528,10 @@
         <v>0</v>
       </c>
       <c r="B70" t="s">
-        <v>69</v>
+        <v>146</v>
       </c>
       <c r="C70" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -2516,10 +2539,10 @@
         <v>0</v>
       </c>
       <c r="B71" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C71" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -2527,7 +2550,7 @@
         <v>0</v>
       </c>
       <c r="B72" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C72" t="s">
         <v>131</v>
@@ -2538,10 +2561,10 @@
         <v>0</v>
       </c>
       <c r="B73" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C73" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -2549,51 +2572,51 @@
         <v>0</v>
       </c>
       <c r="B74" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C74" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
-        <v>144</v>
+        <v>0</v>
       </c>
       <c r="B75" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C75" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
-        <v>144</v>
+        <v>0</v>
       </c>
       <c r="B76" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C76" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
-        <v>144</v>
+        <v>0</v>
       </c>
       <c r="B77" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C77" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B78" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C78" t="s">
         <v>130</v>
@@ -2601,10 +2624,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B79" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C79" t="s">
         <v>130</v>
@@ -2612,10 +2635,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B80" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C80" t="s">
         <v>130</v>
@@ -2623,10 +2646,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B81" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C81" t="s">
         <v>130</v>
@@ -2634,10 +2657,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B82" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C82" t="s">
         <v>130</v>
@@ -2645,10 +2668,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B83" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C83" t="s">
         <v>130</v>
@@ -2656,10 +2679,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B84" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C84" t="s">
         <v>130</v>
@@ -2667,10 +2690,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B85" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C85" t="s">
         <v>130</v>
@@ -2678,10 +2701,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B86" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C86" t="s">
         <v>130</v>
@@ -2689,10 +2712,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B87" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C87" t="s">
         <v>130</v>
@@ -2700,10 +2723,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B88" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C88" t="s">
         <v>130</v>
@@ -2711,10 +2734,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B89" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C89" t="s">
         <v>130</v>
@@ -2722,10 +2745,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B90" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C90" t="s">
         <v>130</v>
@@ -2733,10 +2756,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B91" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C91" t="s">
         <v>130</v>
@@ -2744,10 +2767,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B92" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C92" t="s">
         <v>130</v>
@@ -2755,10 +2778,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B93" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C93" t="s">
         <v>130</v>
@@ -2766,10 +2789,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B94" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C94" t="s">
         <v>130</v>
@@ -2777,21 +2800,21 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B95" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C95" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B96" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C96" t="s">
         <v>130</v>
@@ -2799,10 +2822,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B97" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C97" t="s">
         <v>130</v>
@@ -2810,21 +2833,21 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B98" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C98" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B99" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C99" t="s">
         <v>130</v>
@@ -2832,10 +2855,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B100" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C100" t="s">
         <v>130</v>
@@ -2843,10 +2866,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B101" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C101" t="s">
         <v>130</v>
@@ -2854,10 +2877,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B102" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C102" t="s">
         <v>130</v>
@@ -2865,10 +2888,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B103" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C103" t="s">
         <v>130</v>
@@ -2876,10 +2899,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B104" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C104" t="s">
         <v>130</v>
@@ -2887,10 +2910,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B105" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C105" t="s">
         <v>130</v>
@@ -2898,10 +2921,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B106" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C106" t="s">
         <v>130</v>
@@ -2909,10 +2932,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B107" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C107" t="s">
         <v>130</v>
@@ -2920,10 +2943,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B108" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C108" t="s">
         <v>130</v>
@@ -2931,10 +2954,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B109" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C109" t="s">
         <v>130</v>
@@ -2942,43 +2965,43 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B110" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C110" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B111" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C111" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B112" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C112" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B113" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C113" t="s">
         <v>136</v>
@@ -2986,10 +3009,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B114" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C114" t="s">
         <v>136</v>
@@ -2997,10 +3020,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B115" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C115" t="s">
         <v>136</v>
@@ -3008,10 +3031,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B116" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C116" t="s">
         <v>136</v>
@@ -3019,10 +3042,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B117" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C117" t="s">
         <v>136</v>
@@ -3030,10 +3053,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B118" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C118" t="s">
         <v>136</v>
@@ -3041,10 +3064,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B119" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C119" t="s">
         <v>136</v>
@@ -3052,10 +3075,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B120" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C120" t="s">
         <v>136</v>
@@ -3063,10 +3086,10 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B121" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C121" t="s">
         <v>136</v>
@@ -3074,10 +3097,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B122" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C122" t="s">
         <v>136</v>
@@ -3085,10 +3108,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B123" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C123" t="s">
         <v>136</v>
@@ -3096,83 +3119,116 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B124" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C124" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B125" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C125" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B126" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C126" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B127" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C127" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B128" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C128" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B129" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C129" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B130" t="s">
+        <v>126</v>
+      </c>
+      <c r="C130" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A131" t="s">
+        <v>143</v>
+      </c>
+      <c r="B131" t="s">
+        <v>127</v>
+      </c>
+      <c r="C131" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A132" t="s">
+        <v>143</v>
+      </c>
+      <c r="B132" t="s">
+        <v>128</v>
+      </c>
+      <c r="C132" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133" t="s">
+        <v>143</v>
+      </c>
+      <c r="B133" t="s">
         <v>129</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C133" t="s">
         <v>132</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D130" xr:uid="{C69EDCCF-BBE4-4988-BD44-ED3F6C7FAE7E}"/>
+  <autoFilter ref="A1:D133" xr:uid="{C69EDCCF-BBE4-4988-BD44-ED3F6C7FAE7E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Work on MQ Client
</commit_message>
<xml_diff>
--- a/doc/Functions.xlsx
+++ b/doc/Functions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CurrentProjects\CP4I\Installation\cp4i-install\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01902BFC-3B52-4A3F-B60F-FA0CC329DC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3271933D-279F-42BB-813C-B861F8AA8534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51024" yWindow="1704" windowWidth="21828" windowHeight="12948" tabRatio="483" xr2:uid="{1B9FF1CA-3A2B-40EE-98A9-4DCC44A71825}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="483" xr2:uid="{1B9FF1CA-3A2B-40EE-98A9-4DCC44A71825}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId2"/>
+    <pivotCache cacheId="2" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1258,7 +1258,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{84E5FE0C-A8DF-4E88-AA47-A1A75C172A4E}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{84E5FE0C-A8DF-4E88-AA47-A1A75C172A4E}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F3:I10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisCol" showAll="0">
@@ -1653,11 +1653,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C69EDCCF-BBE4-4988-BD44-ED3F6C7FAE7E}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C68" sqref="C68:C93"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B132" sqref="B132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1688,7 +1689,7 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1699,7 +1700,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1716,7 +1717,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1739,7 +1740,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1762,7 +1763,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1782,7 +1783,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1805,7 +1806,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1828,7 +1829,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1851,7 +1852,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1874,7 +1875,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1885,7 +1886,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1896,7 +1897,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1907,7 +1908,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1918,7 +1919,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1929,7 +1930,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1940,7 +1941,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1951,7 +1952,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1962,7 +1963,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1973,7 +1974,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1984,7 +1985,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1995,7 +1996,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -2006,7 +2007,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -2017,7 +2018,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -2039,7 +2040,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -2050,7 +2051,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -2061,7 +2062,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -2138,7 +2139,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -2160,7 +2161,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -2171,7 +2172,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -2259,7 +2260,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -2281,7 +2282,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>0</v>
       </c>
@@ -2292,7 +2293,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>0</v>
       </c>
@@ -2303,7 +2304,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>0</v>
       </c>
@@ -2314,7 +2315,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>0</v>
       </c>
@@ -2325,7 +2326,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>0</v>
       </c>
@@ -2336,7 +2337,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -2347,7 +2348,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>0</v>
       </c>
@@ -2380,7 +2381,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -2391,7 +2392,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>0</v>
       </c>
@@ -2402,7 +2403,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
         <v>0</v>
       </c>
@@ -2424,7 +2425,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>0</v>
       </c>
@@ -2435,7 +2436,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>0</v>
       </c>
@@ -2446,7 +2447,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
         <v>0</v>
       </c>
@@ -2457,7 +2458,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>0</v>
       </c>
@@ -2468,7 +2469,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
         <v>0</v>
       </c>
@@ -2501,7 +2502,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
         <v>0</v>
       </c>
@@ -2512,7 +2513,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
         <v>0</v>
       </c>
@@ -2523,7 +2524,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
         <v>0</v>
       </c>
@@ -2534,7 +2535,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
         <v>0</v>
       </c>
@@ -2545,7 +2546,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
         <v>0</v>
       </c>
@@ -2567,7 +2568,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
         <v>0</v>
       </c>
@@ -2578,7 +2579,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
         <v>0</v>
       </c>
@@ -2589,7 +2590,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
         <v>0</v>
       </c>
@@ -2611,7 +2612,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
         <v>143</v>
       </c>
@@ -2622,7 +2623,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
         <v>143</v>
       </c>
@@ -2633,7 +2634,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
         <v>143</v>
       </c>
@@ -2644,7 +2645,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
         <v>143</v>
       </c>
@@ -2655,7 +2656,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
         <v>143</v>
       </c>
@@ -2666,7 +2667,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
         <v>143</v>
       </c>
@@ -2677,7 +2678,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
         <v>143</v>
       </c>
@@ -2688,7 +2689,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
         <v>143</v>
       </c>
@@ -2699,7 +2700,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
         <v>143</v>
       </c>
@@ -2710,7 +2711,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
         <v>143</v>
       </c>
@@ -2721,7 +2722,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
         <v>143</v>
       </c>
@@ -2732,7 +2733,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
         <v>143</v>
       </c>
@@ -2743,7 +2744,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
         <v>143</v>
       </c>
@@ -2754,7 +2755,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
         <v>143</v>
       </c>
@@ -2765,7 +2766,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
         <v>143</v>
       </c>
@@ -2776,7 +2777,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
         <v>143</v>
       </c>
@@ -2787,7 +2788,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
         <v>143</v>
       </c>
@@ -2798,7 +2799,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
         <v>143</v>
       </c>
@@ -2809,7 +2810,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
         <v>143</v>
       </c>
@@ -2820,7 +2821,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
         <v>143</v>
       </c>
@@ -2831,7 +2832,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
         <v>143</v>
       </c>
@@ -2842,7 +2843,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
         <v>143</v>
       </c>
@@ -2853,7 +2854,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
         <v>143</v>
       </c>
@@ -2864,7 +2865,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
         <v>143</v>
       </c>
@@ -2875,7 +2876,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
         <v>143</v>
       </c>
@@ -2886,7 +2887,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
         <v>143</v>
       </c>
@@ -2897,7 +2898,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
         <v>143</v>
       </c>
@@ -2908,7 +2909,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
         <v>143</v>
       </c>
@@ -2919,7 +2920,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
         <v>143</v>
       </c>
@@ -2930,7 +2931,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
         <v>143</v>
       </c>
@@ -2941,7 +2942,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
         <v>143</v>
       </c>
@@ -2952,7 +2953,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
         <v>143</v>
       </c>
@@ -2963,7 +2964,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
         <v>143</v>
       </c>
@@ -2974,7 +2975,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
         <v>143</v>
       </c>
@@ -2985,7 +2986,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
         <v>143</v>
       </c>
@@ -2996,7 +2997,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
         <v>143</v>
       </c>
@@ -3007,7 +3008,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
         <v>143</v>
       </c>
@@ -3018,7 +3019,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
         <v>143</v>
       </c>
@@ -3029,7 +3030,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
         <v>143</v>
       </c>
@@ -3040,7 +3041,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" t="s">
         <v>143</v>
       </c>
@@ -3051,7 +3052,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" t="s">
         <v>143</v>
       </c>
@@ -3062,7 +3063,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
         <v>143</v>
       </c>
@@ -3073,7 +3074,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
         <v>143</v>
       </c>
@@ -3084,7 +3085,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" t="s">
         <v>143</v>
       </c>
@@ -3095,7 +3096,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="s">
         <v>143</v>
       </c>
@@ -3106,7 +3107,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" t="s">
         <v>143</v>
       </c>
@@ -3117,7 +3118,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="s">
         <v>143</v>
       </c>
@@ -3128,7 +3129,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" t="s">
         <v>143</v>
       </c>
@@ -3139,7 +3140,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="s">
         <v>143</v>
       </c>
@@ -3150,7 +3151,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="s">
         <v>143</v>
       </c>
@@ -3161,7 +3162,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
         <v>143</v>
       </c>
@@ -3172,7 +3173,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
         <v>143</v>
       </c>
@@ -3183,7 +3184,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" t="s">
         <v>143</v>
       </c>
@@ -3194,7 +3195,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
         <v>143</v>
       </c>
@@ -3228,7 +3229,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D133" xr:uid="{C69EDCCF-BBE4-4988-BD44-ED3F6C7FAE7E}"/>
+  <autoFilter ref="A1:D133" xr:uid="{C69EDCCF-BBE4-4988-BD44-ED3F6C7FAE7E}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Util"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Wrok on Milvus adjutments to versions
</commit_message>
<xml_diff>
--- a/doc/Functions.xlsx
+++ b/doc/Functions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CurrentProjects\CP4I\Installation\cp4i-install\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AB3665-10CD-47AE-8741-59355C390B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4D4FE2-50FF-4E55-BD38-34853F56B8D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5328" yWindow="3696" windowWidth="24996" windowHeight="14136" tabRatio="483" xr2:uid="{1B9FF1CA-3A2B-40EE-98A9-4DCC44A71825}"/>
+    <workbookView xWindow="48312" yWindow="1488" windowWidth="24996" windowHeight="14136" tabRatio="483" xr2:uid="{1B9FF1CA-3A2B-40EE-98A9-4DCC44A71825}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1657,8 +1657,8 @@
   <dimension ref="A1:I133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B64" sqref="B64"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A132" sqref="A132:A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2018,7 +2018,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>0</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>0</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>0</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>0</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>0</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>0</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>0</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
         <v>0</v>
       </c>
@@ -2458,7 +2458,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>0</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>0</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>0</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
         <v>0</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
         <v>0</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="132" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="s">
         <v>143</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="133" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" t="s">
         <v>143</v>
       </c>
@@ -3230,12 +3230,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:D133" xr:uid="{C69EDCCF-BBE4-4988-BD44-ED3F6C7FAE7E}">
-    <filterColumn colId="1">
+    <filterColumn colId="2">
       <filters>
-        <filter val="wait_for_catalogsource_2be_ready"/>
-        <filter val="wait_for_resource"/>
-        <filter val="wait_for_state"/>
-        <filter val="waitn"/>
+        <filter val="Util"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Work in progress for APIC V12
</commit_message>
<xml_diff>
--- a/doc/Functions.xlsx
+++ b/doc/Functions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CurrentProjects\CP4I\Installation\cp4i-install\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4D4FE2-50FF-4E55-BD38-34853F56B8D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B421B9-9E12-4FB9-B934-6EEE27159946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48312" yWindow="1488" windowWidth="24996" windowHeight="14136" tabRatio="483" xr2:uid="{1B9FF1CA-3A2B-40EE-98A9-4DCC44A71825}"/>
+    <workbookView xWindow="49776" yWindow="936" windowWidth="24144" windowHeight="14388" tabRatio="483" xr2:uid="{1B9FF1CA-3A2B-40EE-98A9-4DCC44A71825}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId2"/>
+    <pivotCache cacheId="7" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -526,13 +526,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1258,7 +1259,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{84E5FE0C-A8DF-4E88-AA47-A1A75C172A4E}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{84E5FE0C-A8DF-4E88-AA47-A1A75C172A4E}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F3:I10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisCol" showAll="0">
@@ -1653,12 +1654,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C69EDCCF-BBE4-4988-BD44-ED3F6C7FAE7E}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A132" sqref="A132:A133"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>0</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>0</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>0</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>0</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>0</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>0</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>0</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
         <v>0</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>0</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>0</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
         <v>0</v>
       </c>
@@ -2458,7 +2458,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>0</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
         <v>0</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
         <v>0</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
         <v>0</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
         <v>0</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
         <v>0</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
         <v>0</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
         <v>0</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
         <v>0</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
         <v>0</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
         <v>143</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
         <v>143</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
         <v>143</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
         <v>143</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
         <v>143</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
         <v>143</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
         <v>143</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="85" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
         <v>143</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
         <v>143</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
         <v>143</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="88" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
         <v>143</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="89" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
         <v>143</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
         <v>143</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="91" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
         <v>143</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="92" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
         <v>143</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
         <v>143</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
         <v>143</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="95" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
         <v>143</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="96" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
         <v>143</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
         <v>143</v>
       </c>
@@ -2832,7 +2832,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
         <v>143</v>
       </c>
@@ -2842,8 +2842,9 @@
       <c r="C98" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D98" s="4"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
         <v>143</v>
       </c>
@@ -2854,7 +2855,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
         <v>143</v>
       </c>
@@ -2865,7 +2866,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
         <v>143</v>
       </c>
@@ -2876,7 +2877,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
         <v>143</v>
       </c>
@@ -2887,7 +2888,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
         <v>143</v>
       </c>
@@ -2898,7 +2899,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
         <v>143</v>
       </c>
@@ -2909,7 +2910,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
         <v>143</v>
       </c>
@@ -2920,7 +2921,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
         <v>143</v>
       </c>
@@ -2931,7 +2932,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
         <v>143</v>
       </c>
@@ -2942,7 +2943,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
         <v>143</v>
       </c>
@@ -2953,7 +2954,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
         <v>143</v>
       </c>
@@ -2964,7 +2965,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
         <v>143</v>
       </c>
@@ -2975,7 +2976,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
         <v>143</v>
       </c>
@@ -2986,7 +2987,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
         <v>143</v>
       </c>
@@ -2997,7 +2998,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="113" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
         <v>143</v>
       </c>
@@ -3008,7 +3009,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="114" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
         <v>143</v>
       </c>
@@ -3019,7 +3020,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
         <v>143</v>
       </c>
@@ -3030,7 +3031,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="116" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
         <v>143</v>
       </c>
@@ -3041,7 +3042,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="117" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" t="s">
         <v>143</v>
       </c>
@@ -3052,7 +3053,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="118" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" t="s">
         <v>143</v>
       </c>
@@ -3063,7 +3064,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="119" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
         <v>143</v>
       </c>
@@ -3074,7 +3075,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="120" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
         <v>143</v>
       </c>
@@ -3085,7 +3086,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="121" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" t="s">
         <v>143</v>
       </c>
@@ -3096,7 +3097,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="122" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="s">
         <v>143</v>
       </c>
@@ -3107,7 +3108,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="123" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" t="s">
         <v>143</v>
       </c>
@@ -3118,7 +3119,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="124" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="s">
         <v>143</v>
       </c>
@@ -3129,7 +3130,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="125" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" t="s">
         <v>143</v>
       </c>
@@ -3140,7 +3141,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="126" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="s">
         <v>143</v>
       </c>
@@ -3151,7 +3152,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="127" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="s">
         <v>143</v>
       </c>
@@ -3162,7 +3163,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="128" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
         <v>143</v>
       </c>
@@ -3173,7 +3174,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="129" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
         <v>143</v>
       </c>
@@ -3184,7 +3185,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="130" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" t="s">
         <v>143</v>
       </c>
@@ -3195,7 +3196,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="131" spans="1:3" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
         <v>143</v>
       </c>
@@ -3229,13 +3230,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D133" xr:uid="{C69EDCCF-BBE4-4988-BD44-ED3F6C7FAE7E}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Util"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:D133" xr:uid="{C69EDCCF-BBE4-4988-BD44-ED3F6C7FAE7E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>